<commit_message>
address the validation issue #11; addressed in the memo #1
</commit_message>
<xml_diff>
--- a/data-raw/survey_info_macrointerest.xlsx
+++ b/data-raw/survey_info_macrointerest.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E614"/>
+  <dimension ref="A1:F614"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,15 +370,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>creator</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>link</t>
         </is>

</xml_diff>